<commit_message>
Adding number formats & column widths
Adding the ability to choose different number formats for numeric and formula cells as well as the ability to set custom column widths.
</commit_message>
<xml_diff>
--- a/BasicWorkbook/test1.xlsx
+++ b/BasicWorkbook/test1.xlsx
@@ -11,6 +11,59 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <numFmts count="51">
+    <numFmt numFmtId="100" formatCode="0"/>
+    <numFmt numFmtId="101" formatCode="0.0"/>
+    <numFmt numFmtId="102" formatCode="0.00"/>
+    <numFmt numFmtId="103" formatCode="0.000"/>
+    <numFmt numFmtId="104" formatCode="0.0000"/>
+    <numFmt numFmtId="105" formatCode="0.00000"/>
+    <numFmt numFmtId="106" formatCode="0.000000"/>
+    <numFmt numFmtId="107" formatCode="0.0000000"/>
+    <numFmt numFmtId="108" formatCode="0.00000000"/>
+    <numFmt numFmtId="109" formatCode="0.000000000"/>
+    <numFmt numFmtId="110" formatCode="0.0000000000"/>
+    <numFmt numFmtId="111" formatCode="0.00000000000"/>
+    <numFmt numFmtId="112" formatCode="0.000000000000"/>
+    <numFmt numFmtId="113" formatCode="0.0000000000000"/>
+    <numFmt numFmtId="114" formatCode="0.00000000000000"/>
+    <numFmt numFmtId="115" formatCode="0.000000000000000"/>
+    <numFmt numFmtId="116" formatCode="0.0000000000000000"/>
+    <numFmt numFmtId="117" formatCode="0E+0"/>
+    <numFmt numFmtId="118" formatCode="0.0E+0"/>
+    <numFmt numFmtId="119" formatCode="0.00E+0"/>
+    <numFmt numFmtId="120" formatCode="0.000E+0"/>
+    <numFmt numFmtId="121" formatCode="0.0000E+0"/>
+    <numFmt numFmtId="122" formatCode="0.00000E+0"/>
+    <numFmt numFmtId="123" formatCode="0.000000E+0"/>
+    <numFmt numFmtId="124" formatCode="0.0000000E+0"/>
+    <numFmt numFmtId="125" formatCode="0.00000000E+0"/>
+    <numFmt numFmtId="126" formatCode="0.000000000E+0"/>
+    <numFmt numFmtId="127" formatCode="0.0000000000E+0"/>
+    <numFmt numFmtId="128" formatCode="0.00000000000E+0"/>
+    <numFmt numFmtId="129" formatCode="0.000000000000E+0"/>
+    <numFmt numFmtId="130" formatCode="0.0000000000000E+0"/>
+    <numFmt numFmtId="131" formatCode="0.00000000000000E+0"/>
+    <numFmt numFmtId="132" formatCode="0.000000000000000E+0"/>
+    <numFmt numFmtId="133" formatCode="0.0000000000000000E+0"/>
+    <numFmt numFmtId="134" formatCode="0%"/>
+    <numFmt numFmtId="135" formatCode="0.0%"/>
+    <numFmt numFmtId="136" formatCode="0.00%"/>
+    <numFmt numFmtId="137" formatCode="0.000%"/>
+    <numFmt numFmtId="138" formatCode="0.0000%"/>
+    <numFmt numFmtId="139" formatCode="0.00000%"/>
+    <numFmt numFmtId="140" formatCode="0.000000%"/>
+    <numFmt numFmtId="141" formatCode="0.0000000%"/>
+    <numFmt numFmtId="142" formatCode="0.00000000%"/>
+    <numFmt numFmtId="143" formatCode="0.000000000%"/>
+    <numFmt numFmtId="144" formatCode="0.0000000000%"/>
+    <numFmt numFmtId="145" formatCode="0.00000000000%"/>
+    <numFmt numFmtId="146" formatCode="0.000000000000%"/>
+    <numFmt numFmtId="147" formatCode="0.0000000000000%"/>
+    <numFmt numFmtId="148" formatCode="0.00000000000000%"/>
+    <numFmt numFmtId="149" formatCode="0.000000000000000%"/>
+    <numFmt numFmtId="150" formatCode="0.0000000000000000%"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <sz val="12"/>
@@ -37,8 +90,60 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="53">
+    <xf numFmtId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="100" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="101" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="102" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="103" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="104" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="105" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="106" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="107" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="108" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="109" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="110" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="111" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="112" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="113" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="114" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="115" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="116" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="117" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="118" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="119" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="120" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="121" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="122" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="123" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="124" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="125" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="126" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="127" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="128" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="129" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="130" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="131" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="132" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="133" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="134" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="135" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="136" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="137" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="138" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="139" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="140" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="141" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="142" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="143" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="144" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="145" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="146" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="147" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="148" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="149" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="150" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -54,19 +159,24 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17"/>
+  <cols>
+    <col min="1" max="1" width="9.005" bestFit="1"/>
+    <col min="2" max="2" width="9.005" bestFit="1"/>
+    <col min="3" max="3" width="9.005" bestFit="1"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="52" t="inlineStr">
         <is>
           <t>col 1</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="52" t="inlineStr">
         <is>
           <t>col 2</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="52" t="inlineStr">
         <is>
           <t>col 3</t>
         </is>
@@ -115,19 +225,24 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17"/>
+  <cols>
+    <col min="1" max="1" width="9.005" bestFit="1"/>
+    <col min="2" max="2" width="9.005" bestFit="1"/>
+    <col min="3" max="3" width="9.005" bestFit="1"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="52" t="inlineStr">
         <is>
           <t>col 1</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="52" t="inlineStr">
         <is>
           <t>col 2</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="52" t="inlineStr">
         <is>
           <t>col 3</t>
         </is>
@@ -1234,7 +1349,7 @@
       </c>
     </row>
     <row r="102">
-      <c r="B102" t="inlineStr">
+      <c r="B102" s="52" t="inlineStr">
         <is>
           <t>total:</t>
         </is>

</xml_diff>

<commit_message>
Adding merged cells, more formatting, makefiles
Fixed errors that prevented compilation with g++.
Added makefiles for nmake and unix make.
BasicWorkbook now supports merged cells (presently for text only, numbers & formulas to follow), bold text, wrapped text, and different options for vertical and horizontal alignment of the value in the cell.
</commit_message>
<xml_diff>
--- a/BasicWorkbook/test1.xlsx
+++ b/BasicWorkbook/test1.xlsx
@@ -64,8 +64,16 @@
     <numFmt numFmtId="149" formatCode="0.000000000000000%"/>
     <numFmt numFmtId="150" formatCode="0.0000000000000000%"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -90,60 +98,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
-    <xf numFmtId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="100" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="101" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="102" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="103" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="104" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="105" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="106" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="107" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="108" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="109" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="110" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="111" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="112" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="113" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="114" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="115" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="116" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="117" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="118" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="119" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="120" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="121" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="122" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="123" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="124" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="125" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="126" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="127" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="128" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="129" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="130" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="131" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="132" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="133" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="134" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="135" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="136" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="137" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="138" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="139" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="140" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="141" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="142" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="143" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="144" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="145" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="146" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="147" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="148" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="149" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="150" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="3">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" wrapText="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="general" vertical="bottom" wrapText="false"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="bottom" wrapText="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -166,52 +130,52 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="52" t="inlineStr">
+      <c r="A1" s="0" t="inlineStr">
         <is>
           <t>col 1</t>
         </is>
       </c>
-      <c r="B1" s="52" t="inlineStr">
+      <c r="B1" s="0" t="inlineStr">
         <is>
           <t>col 2</t>
         </is>
       </c>
-      <c r="C1" s="52" t="inlineStr">
+      <c r="C1" s="0" t="inlineStr">
         <is>
           <t>col 3</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>1.000000</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>4.000000</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <f>A2+B2</f>
       </c>
     </row>
     <row r="3">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>2.000000</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>5.000000</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <f>A3+B3</f>
       </c>
     </row>
     <row r="4">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>3.000000</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>6.000000</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <f>A4+B4</f>
       </c>
     </row>
@@ -232,1132 +196,1136 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="52" t="inlineStr">
+      <c r="A1" s="0" t="inlineStr">
         <is>
           <t>col 1</t>
         </is>
       </c>
-      <c r="B1" s="52" t="inlineStr">
+      <c r="B1" s="0" t="inlineStr">
         <is>
           <t>col 2</t>
         </is>
       </c>
-      <c r="C1" s="52" t="inlineStr">
+      <c r="C1" s="0" t="inlineStr">
         <is>
           <t>col 3</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>1.000000</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>2.000000</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <f>A2+B2</f>
       </c>
     </row>
     <row r="3">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>2.000000</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>3.000000</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <f>A3+B3</f>
       </c>
     </row>
     <row r="4">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>3.000000</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>4.000000</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <f>A4+B4</f>
       </c>
     </row>
     <row r="5">
-      <c r="A5">
+      <c r="A5" s="1">
         <v>4.000000</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>5.000000</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <f>A5+B5</f>
       </c>
     </row>
     <row r="6">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>5.000000</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>6.000000</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <f>A6+B6</f>
       </c>
     </row>
     <row r="7">
-      <c r="A7">
+      <c r="A7" s="1">
         <v>6.000000</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>7.000000</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <f>A7+B7</f>
       </c>
     </row>
     <row r="8">
-      <c r="A8">
+      <c r="A8" s="1">
         <v>7.000000</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>8.000000</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <f>A8+B8</f>
       </c>
     </row>
     <row r="9">
-      <c r="A9">
+      <c r="A9" s="1">
         <v>8.000000</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>9.000000</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <f>A9+B9</f>
       </c>
     </row>
     <row r="10">
-      <c r="A10">
+      <c r="A10" s="1">
         <v>9.000000</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>10.000000</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="1">
         <f>A10+B10</f>
       </c>
     </row>
     <row r="11">
-      <c r="A11">
+      <c r="A11" s="1">
         <v>10.000000</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>11.000000</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <f>A11+B11</f>
       </c>
     </row>
     <row r="12">
-      <c r="A12">
+      <c r="A12" s="1">
         <v>11.000000</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
         <v>12.000000</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
         <f>A12+B12</f>
       </c>
     </row>
     <row r="13">
-      <c r="A13">
+      <c r="A13" s="1">
         <v>12.000000</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
         <v>13.000000</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <f>A13+B13</f>
       </c>
     </row>
     <row r="14">
-      <c r="A14">
+      <c r="A14" s="1">
         <v>13.000000</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1">
         <v>14.000000</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="1">
         <f>A14+B14</f>
       </c>
     </row>
     <row r="15">
-      <c r="A15">
+      <c r="A15" s="1">
         <v>14.000000</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="1">
         <v>15.000000</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="1">
         <f>A15+B15</f>
       </c>
     </row>
     <row r="16">
-      <c r="A16">
+      <c r="A16" s="1">
         <v>15.000000</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="1">
         <v>16.000000</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="1">
         <f>A16+B16</f>
       </c>
     </row>
     <row r="17">
-      <c r="A17">
+      <c r="A17" s="1">
         <v>16.000000</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="1">
         <v>17.000000</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="1">
         <f>A17+B17</f>
       </c>
     </row>
     <row r="18">
-      <c r="A18">
+      <c r="A18" s="1">
         <v>17.000000</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="1">
         <v>18.000000</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="1">
         <f>A18+B18</f>
       </c>
     </row>
     <row r="19">
-      <c r="A19">
+      <c r="A19" s="1">
         <v>18.000000</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="1">
         <v>19.000000</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="1">
         <f>A19+B19</f>
       </c>
     </row>
     <row r="20">
-      <c r="A20">
+      <c r="A20" s="1">
         <v>19.000000</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="1">
         <v>20.000000</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="1">
         <f>A20+B20</f>
       </c>
     </row>
     <row r="21">
-      <c r="A21">
+      <c r="A21" s="1">
         <v>20.000000</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="1">
         <v>21.000000</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="1">
         <f>A21+B21</f>
       </c>
     </row>
     <row r="22">
-      <c r="A22">
+      <c r="A22" s="1">
         <v>21.000000</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="1">
         <v>22.000000</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="1">
         <f>A22+B22</f>
       </c>
     </row>
     <row r="23">
-      <c r="A23">
+      <c r="A23" s="1">
         <v>22.000000</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="1">
         <v>23.000000</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="1">
         <f>A23+B23</f>
       </c>
     </row>
     <row r="24">
-      <c r="A24">
+      <c r="A24" s="1">
         <v>23.000000</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="1">
         <v>24.000000</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="1">
         <f>A24+B24</f>
       </c>
     </row>
     <row r="25">
-      <c r="A25">
+      <c r="A25" s="1">
         <v>24.000000</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="1">
         <v>25.000000</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="1">
         <f>A25+B25</f>
       </c>
     </row>
     <row r="26">
-      <c r="A26">
+      <c r="A26" s="1">
         <v>25.000000</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="1">
         <v>26.000000</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="1">
         <f>A26+B26</f>
       </c>
     </row>
     <row r="27">
-      <c r="A27">
+      <c r="A27" s="1">
         <v>26.000000</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="1">
         <v>27.000000</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="1">
         <f>A27+B27</f>
       </c>
     </row>
     <row r="28">
-      <c r="A28">
+      <c r="A28" s="1">
         <v>27.000000</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="1">
         <v>28.000000</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="1">
         <f>A28+B28</f>
       </c>
     </row>
     <row r="29">
-      <c r="A29">
+      <c r="A29" s="1">
         <v>28.000000</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="1">
         <v>29.000000</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="1">
         <f>A29+B29</f>
       </c>
     </row>
     <row r="30">
-      <c r="A30">
+      <c r="A30" s="1">
         <v>29.000000</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="1">
         <v>30.000000</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="1">
         <f>A30+B30</f>
       </c>
     </row>
     <row r="31">
-      <c r="A31">
+      <c r="A31" s="1">
         <v>30.000000</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="1">
         <v>31.000000</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="1">
         <f>A31+B31</f>
       </c>
     </row>
     <row r="32">
-      <c r="A32">
+      <c r="A32" s="1">
         <v>31.000000</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="1">
         <v>32.000000</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="1">
         <f>A32+B32</f>
       </c>
     </row>
     <row r="33">
-      <c r="A33">
+      <c r="A33" s="1">
         <v>32.000000</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="1">
         <v>33.000000</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="1">
         <f>A33+B33</f>
       </c>
     </row>
     <row r="34">
-      <c r="A34">
+      <c r="A34" s="1">
         <v>33.000000</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="1">
         <v>34.000000</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="1">
         <f>A34+B34</f>
       </c>
     </row>
     <row r="35">
-      <c r="A35">
+      <c r="A35" s="1">
         <v>34.000000</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="1">
         <v>35.000000</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="1">
         <f>A35+B35</f>
       </c>
     </row>
     <row r="36">
-      <c r="A36">
+      <c r="A36" s="1">
         <v>35.000000</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="1">
         <v>36.000000</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="1">
         <f>A36+B36</f>
       </c>
     </row>
     <row r="37">
-      <c r="A37">
+      <c r="A37" s="1">
         <v>36.000000</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="1">
         <v>37.000000</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="1">
         <f>A37+B37</f>
       </c>
     </row>
     <row r="38">
-      <c r="A38">
+      <c r="A38" s="1">
         <v>37.000000</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="1">
         <v>38.000000</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="1">
         <f>A38+B38</f>
       </c>
     </row>
     <row r="39">
-      <c r="A39">
+      <c r="A39" s="1">
         <v>38.000000</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="1">
         <v>39.000000</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="1">
         <f>A39+B39</f>
       </c>
     </row>
     <row r="40">
-      <c r="A40">
+      <c r="A40" s="1">
         <v>39.000000</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="1">
         <v>40.000000</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="1">
         <f>A40+B40</f>
       </c>
     </row>
     <row r="41">
-      <c r="A41">
+      <c r="A41" s="1">
         <v>40.000000</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="1">
         <v>41.000000</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="1">
         <f>A41+B41</f>
       </c>
     </row>
     <row r="42">
-      <c r="A42">
+      <c r="A42" s="1">
         <v>41.000000</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="1">
         <v>42.000000</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="1">
         <f>A42+B42</f>
       </c>
     </row>
     <row r="43">
-      <c r="A43">
+      <c r="A43" s="1">
         <v>42.000000</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="1">
         <v>43.000000</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="1">
         <f>A43+B43</f>
       </c>
     </row>
     <row r="44">
-      <c r="A44">
+      <c r="A44" s="1">
         <v>43.000000</v>
       </c>
-      <c r="B44">
+      <c r="B44" s="1">
         <v>44.000000</v>
       </c>
-      <c r="C44">
+      <c r="C44" s="1">
         <f>A44+B44</f>
       </c>
     </row>
     <row r="45">
-      <c r="A45">
+      <c r="A45" s="1">
         <v>44.000000</v>
       </c>
-      <c r="B45">
+      <c r="B45" s="1">
         <v>45.000000</v>
       </c>
-      <c r="C45">
+      <c r="C45" s="1">
         <f>A45+B45</f>
       </c>
     </row>
     <row r="46">
-      <c r="A46">
+      <c r="A46" s="1">
         <v>45.000000</v>
       </c>
-      <c r="B46">
+      <c r="B46" s="1">
         <v>46.000000</v>
       </c>
-      <c r="C46">
+      <c r="C46" s="1">
         <f>A46+B46</f>
       </c>
     </row>
     <row r="47">
-      <c r="A47">
+      <c r="A47" s="1">
         <v>46.000000</v>
       </c>
-      <c r="B47">
+      <c r="B47" s="1">
         <v>47.000000</v>
       </c>
-      <c r="C47">
+      <c r="C47" s="1">
         <f>A47+B47</f>
       </c>
     </row>
     <row r="48">
-      <c r="A48">
+      <c r="A48" s="1">
         <v>47.000000</v>
       </c>
-      <c r="B48">
+      <c r="B48" s="1">
         <v>48.000000</v>
       </c>
-      <c r="C48">
+      <c r="C48" s="1">
         <f>A48+B48</f>
       </c>
     </row>
     <row r="49">
-      <c r="A49">
+      <c r="A49" s="1">
         <v>48.000000</v>
       </c>
-      <c r="B49">
+      <c r="B49" s="1">
         <v>49.000000</v>
       </c>
-      <c r="C49">
+      <c r="C49" s="1">
         <f>A49+B49</f>
       </c>
     </row>
     <row r="50">
-      <c r="A50">
+      <c r="A50" s="1">
         <v>49.000000</v>
       </c>
-      <c r="B50">
+      <c r="B50" s="1">
         <v>50.000000</v>
       </c>
-      <c r="C50">
+      <c r="C50" s="1">
         <f>A50+B50</f>
       </c>
     </row>
     <row r="51">
-      <c r="A51">
+      <c r="A51" s="1">
         <v>50.000000</v>
       </c>
-      <c r="B51">
+      <c r="B51" s="1">
         <v>51.000000</v>
       </c>
-      <c r="C51">
+      <c r="C51" s="1">
         <f>A51+B51</f>
       </c>
     </row>
     <row r="52">
-      <c r="A52">
+      <c r="A52" s="1">
         <v>51.000000</v>
       </c>
-      <c r="B52">
+      <c r="B52" s="1">
         <v>52.000000</v>
       </c>
-      <c r="C52">
+      <c r="C52" s="1">
         <f>A52+B52</f>
       </c>
     </row>
     <row r="53">
-      <c r="A53">
+      <c r="A53" s="1">
         <v>52.000000</v>
       </c>
-      <c r="B53">
+      <c r="B53" s="1">
         <v>53.000000</v>
       </c>
-      <c r="C53">
+      <c r="C53" s="1">
         <f>A53+B53</f>
       </c>
     </row>
     <row r="54">
-      <c r="A54">
+      <c r="A54" s="1">
         <v>53.000000</v>
       </c>
-      <c r="B54">
+      <c r="B54" s="1">
         <v>54.000000</v>
       </c>
-      <c r="C54">
+      <c r="C54" s="1">
         <f>A54+B54</f>
       </c>
     </row>
     <row r="55">
-      <c r="A55">
+      <c r="A55" s="1">
         <v>54.000000</v>
       </c>
-      <c r="B55">
+      <c r="B55" s="1">
         <v>55.000000</v>
       </c>
-      <c r="C55">
+      <c r="C55" s="1">
         <f>A55+B55</f>
       </c>
     </row>
     <row r="56">
-      <c r="A56">
+      <c r="A56" s="1">
         <v>55.000000</v>
       </c>
-      <c r="B56">
+      <c r="B56" s="1">
         <v>56.000000</v>
       </c>
-      <c r="C56">
+      <c r="C56" s="1">
         <f>A56+B56</f>
       </c>
     </row>
     <row r="57">
-      <c r="A57">
+      <c r="A57" s="1">
         <v>56.000000</v>
       </c>
-      <c r="B57">
+      <c r="B57" s="1">
         <v>57.000000</v>
       </c>
-      <c r="C57">
+      <c r="C57" s="1">
         <f>A57+B57</f>
       </c>
     </row>
     <row r="58">
-      <c r="A58">
+      <c r="A58" s="1">
         <v>57.000000</v>
       </c>
-      <c r="B58">
+      <c r="B58" s="1">
         <v>58.000000</v>
       </c>
-      <c r="C58">
+      <c r="C58" s="1">
         <f>A58+B58</f>
       </c>
     </row>
     <row r="59">
-      <c r="A59">
+      <c r="A59" s="1">
         <v>58.000000</v>
       </c>
-      <c r="B59">
+      <c r="B59" s="1">
         <v>59.000000</v>
       </c>
-      <c r="C59">
+      <c r="C59" s="1">
         <f>A59+B59</f>
       </c>
     </row>
     <row r="60">
-      <c r="A60">
+      <c r="A60" s="1">
         <v>59.000000</v>
       </c>
-      <c r="B60">
+      <c r="B60" s="1">
         <v>60.000000</v>
       </c>
-      <c r="C60">
+      <c r="C60" s="1">
         <f>A60+B60</f>
       </c>
     </row>
     <row r="61">
-      <c r="A61">
+      <c r="A61" s="1">
         <v>60.000000</v>
       </c>
-      <c r="B61">
+      <c r="B61" s="1">
         <v>61.000000</v>
       </c>
-      <c r="C61">
+      <c r="C61" s="1">
         <f>A61+B61</f>
       </c>
     </row>
     <row r="62">
-      <c r="A62">
+      <c r="A62" s="1">
         <v>61.000000</v>
       </c>
-      <c r="B62">
+      <c r="B62" s="1">
         <v>62.000000</v>
       </c>
-      <c r="C62">
+      <c r="C62" s="1">
         <f>A62+B62</f>
       </c>
     </row>
     <row r="63">
-      <c r="A63">
+      <c r="A63" s="1">
         <v>62.000000</v>
       </c>
-      <c r="B63">
+      <c r="B63" s="1">
         <v>63.000000</v>
       </c>
-      <c r="C63">
+      <c r="C63" s="1">
         <f>A63+B63</f>
       </c>
     </row>
     <row r="64">
-      <c r="A64">
+      <c r="A64" s="1">
         <v>63.000000</v>
       </c>
-      <c r="B64">
+      <c r="B64" s="1">
         <v>64.000000</v>
       </c>
-      <c r="C64">
+      <c r="C64" s="1">
         <f>A64+B64</f>
       </c>
     </row>
     <row r="65">
-      <c r="A65">
+      <c r="A65" s="1">
         <v>64.000000</v>
       </c>
-      <c r="B65">
+      <c r="B65" s="1">
         <v>65.000000</v>
       </c>
-      <c r="C65">
+      <c r="C65" s="1">
         <f>A65+B65</f>
       </c>
     </row>
     <row r="66">
-      <c r="A66">
+      <c r="A66" s="1">
         <v>65.000000</v>
       </c>
-      <c r="B66">
+      <c r="B66" s="1">
         <v>66.000000</v>
       </c>
-      <c r="C66">
+      <c r="C66" s="1">
         <f>A66+B66</f>
       </c>
     </row>
     <row r="67">
-      <c r="A67">
+      <c r="A67" s="1">
         <v>66.000000</v>
       </c>
-      <c r="B67">
+      <c r="B67" s="1">
         <v>67.000000</v>
       </c>
-      <c r="C67">
+      <c r="C67" s="1">
         <f>A67+B67</f>
       </c>
     </row>
     <row r="68">
-      <c r="A68">
+      <c r="A68" s="1">
         <v>67.000000</v>
       </c>
-      <c r="B68">
+      <c r="B68" s="1">
         <v>68.000000</v>
       </c>
-      <c r="C68">
+      <c r="C68" s="1">
         <f>A68+B68</f>
       </c>
     </row>
     <row r="69">
-      <c r="A69">
+      <c r="A69" s="1">
         <v>68.000000</v>
       </c>
-      <c r="B69">
+      <c r="B69" s="1">
         <v>69.000000</v>
       </c>
-      <c r="C69">
+      <c r="C69" s="1">
         <f>A69+B69</f>
       </c>
     </row>
     <row r="70">
-      <c r="A70">
+      <c r="A70" s="1">
         <v>69.000000</v>
       </c>
-      <c r="B70">
+      <c r="B70" s="1">
         <v>70.000000</v>
       </c>
-      <c r="C70">
+      <c r="C70" s="1">
         <f>A70+B70</f>
       </c>
     </row>
     <row r="71">
-      <c r="A71">
+      <c r="A71" s="1">
         <v>70.000000</v>
       </c>
-      <c r="B71">
+      <c r="B71" s="1">
         <v>71.000000</v>
       </c>
-      <c r="C71">
+      <c r="C71" s="1">
         <f>A71+B71</f>
       </c>
     </row>
     <row r="72">
-      <c r="A72">
+      <c r="A72" s="1">
         <v>71.000000</v>
       </c>
-      <c r="B72">
+      <c r="B72" s="1">
         <v>72.000000</v>
       </c>
-      <c r="C72">
+      <c r="C72" s="1">
         <f>A72+B72</f>
       </c>
     </row>
     <row r="73">
-      <c r="A73">
+      <c r="A73" s="1">
         <v>72.000000</v>
       </c>
-      <c r="B73">
+      <c r="B73" s="1">
         <v>73.000000</v>
       </c>
-      <c r="C73">
+      <c r="C73" s="1">
         <f>A73+B73</f>
       </c>
     </row>
     <row r="74">
-      <c r="A74">
+      <c r="A74" s="1">
         <v>73.000000</v>
       </c>
-      <c r="B74">
+      <c r="B74" s="1">
         <v>74.000000</v>
       </c>
-      <c r="C74">
+      <c r="C74" s="1">
         <f>A74+B74</f>
       </c>
     </row>
     <row r="75">
-      <c r="A75">
+      <c r="A75" s="1">
         <v>74.000000</v>
       </c>
-      <c r="B75">
+      <c r="B75" s="1">
         <v>75.000000</v>
       </c>
-      <c r="C75">
+      <c r="C75" s="1">
         <f>A75+B75</f>
       </c>
     </row>
     <row r="76">
-      <c r="A76">
+      <c r="A76" s="1">
         <v>75.000000</v>
       </c>
-      <c r="B76">
+      <c r="B76" s="1">
         <v>76.000000</v>
       </c>
-      <c r="C76">
+      <c r="C76" s="1">
         <f>A76+B76</f>
       </c>
     </row>
     <row r="77">
-      <c r="A77">
+      <c r="A77" s="1">
         <v>76.000000</v>
       </c>
-      <c r="B77">
+      <c r="B77" s="1">
         <v>77.000000</v>
       </c>
-      <c r="C77">
+      <c r="C77" s="1">
         <f>A77+B77</f>
       </c>
     </row>
     <row r="78">
-      <c r="A78">
+      <c r="A78" s="1">
         <v>77.000000</v>
       </c>
-      <c r="B78">
+      <c r="B78" s="1">
         <v>78.000000</v>
       </c>
-      <c r="C78">
+      <c r="C78" s="1">
         <f>A78+B78</f>
       </c>
     </row>
     <row r="79">
-      <c r="A79">
+      <c r="A79" s="1">
         <v>78.000000</v>
       </c>
-      <c r="B79">
+      <c r="B79" s="1">
         <v>79.000000</v>
       </c>
-      <c r="C79">
+      <c r="C79" s="1">
         <f>A79+B79</f>
       </c>
     </row>
     <row r="80">
-      <c r="A80">
+      <c r="A80" s="1">
         <v>79.000000</v>
       </c>
-      <c r="B80">
+      <c r="B80" s="1">
         <v>80.000000</v>
       </c>
-      <c r="C80">
+      <c r="C80" s="1">
         <f>A80+B80</f>
       </c>
     </row>
     <row r="81">
-      <c r="A81">
+      <c r="A81" s="1">
         <v>80.000000</v>
       </c>
-      <c r="B81">
+      <c r="B81" s="1">
         <v>81.000000</v>
       </c>
-      <c r="C81">
+      <c r="C81" s="1">
         <f>A81+B81</f>
       </c>
     </row>
     <row r="82">
-      <c r="A82">
+      <c r="A82" s="1">
         <v>81.000000</v>
       </c>
-      <c r="B82">
+      <c r="B82" s="1">
         <v>82.000000</v>
       </c>
-      <c r="C82">
+      <c r="C82" s="1">
         <f>A82+B82</f>
       </c>
     </row>
     <row r="83">
-      <c r="A83">
+      <c r="A83" s="1">
         <v>82.000000</v>
       </c>
-      <c r="B83">
+      <c r="B83" s="1">
         <v>83.000000</v>
       </c>
-      <c r="C83">
+      <c r="C83" s="1">
         <f>A83+B83</f>
       </c>
     </row>
     <row r="84">
-      <c r="A84">
+      <c r="A84" s="1">
         <v>83.000000</v>
       </c>
-      <c r="B84">
+      <c r="B84" s="1">
         <v>84.000000</v>
       </c>
-      <c r="C84">
+      <c r="C84" s="1">
         <f>A84+B84</f>
       </c>
     </row>
     <row r="85">
-      <c r="A85">
+      <c r="A85" s="1">
         <v>84.000000</v>
       </c>
-      <c r="B85">
+      <c r="B85" s="1">
         <v>85.000000</v>
       </c>
-      <c r="C85">
+      <c r="C85" s="1">
         <f>A85+B85</f>
       </c>
     </row>
     <row r="86">
-      <c r="A86">
+      <c r="A86" s="1">
         <v>85.000000</v>
       </c>
-      <c r="B86">
+      <c r="B86" s="1">
         <v>86.000000</v>
       </c>
-      <c r="C86">
+      <c r="C86" s="1">
         <f>A86+B86</f>
       </c>
     </row>
     <row r="87">
-      <c r="A87">
+      <c r="A87" s="1">
         <v>86.000000</v>
       </c>
-      <c r="B87">
+      <c r="B87" s="1">
         <v>87.000000</v>
       </c>
-      <c r="C87">
+      <c r="C87" s="1">
         <f>A87+B87</f>
       </c>
     </row>
     <row r="88">
-      <c r="A88">
+      <c r="A88" s="1">
         <v>87.000000</v>
       </c>
-      <c r="B88">
+      <c r="B88" s="1">
         <v>88.000000</v>
       </c>
-      <c r="C88">
+      <c r="C88" s="1">
         <f>A88+B88</f>
       </c>
     </row>
     <row r="89">
-      <c r="A89">
+      <c r="A89" s="1">
         <v>88.000000</v>
       </c>
-      <c r="B89">
+      <c r="B89" s="1">
         <v>89.000000</v>
       </c>
-      <c r="C89">
+      <c r="C89" s="1">
         <f>A89+B89</f>
       </c>
     </row>
     <row r="90">
-      <c r="A90">
+      <c r="A90" s="1">
         <v>89.000000</v>
       </c>
-      <c r="B90">
+      <c r="B90" s="1">
         <v>90.000000</v>
       </c>
-      <c r="C90">
+      <c r="C90" s="1">
         <f>A90+B90</f>
       </c>
     </row>
     <row r="91">
-      <c r="A91">
+      <c r="A91" s="1">
         <v>90.000000</v>
       </c>
-      <c r="B91">
+      <c r="B91" s="1">
         <v>91.000000</v>
       </c>
-      <c r="C91">
+      <c r="C91" s="1">
         <f>A91+B91</f>
       </c>
     </row>
     <row r="92">
-      <c r="A92">
+      <c r="A92" s="1">
         <v>91.000000</v>
       </c>
-      <c r="B92">
+      <c r="B92" s="1">
         <v>92.000000</v>
       </c>
-      <c r="C92">
+      <c r="C92" s="1">
         <f>A92+B92</f>
       </c>
     </row>
     <row r="93">
-      <c r="A93">
+      <c r="A93" s="1">
         <v>92.000000</v>
       </c>
-      <c r="B93">
+      <c r="B93" s="1">
         <v>93.000000</v>
       </c>
-      <c r="C93">
+      <c r="C93" s="1">
         <f>A93+B93</f>
       </c>
     </row>
     <row r="94">
-      <c r="A94">
+      <c r="A94" s="1">
         <v>93.000000</v>
       </c>
-      <c r="B94">
+      <c r="B94" s="1">
         <v>94.000000</v>
       </c>
-      <c r="C94">
+      <c r="C94" s="1">
         <f>A94+B94</f>
       </c>
     </row>
     <row r="95">
-      <c r="A95">
+      <c r="A95" s="1">
         <v>94.000000</v>
       </c>
-      <c r="B95">
+      <c r="B95" s="1">
         <v>95.000000</v>
       </c>
-      <c r="C95">
+      <c r="C95" s="1">
         <f>A95+B95</f>
       </c>
     </row>
     <row r="96">
-      <c r="A96">
+      <c r="A96" s="1">
         <v>95.000000</v>
       </c>
-      <c r="B96">
+      <c r="B96" s="1">
         <v>96.000000</v>
       </c>
-      <c r="C96">
+      <c r="C96" s="1">
         <f>A96+B96</f>
       </c>
     </row>
     <row r="97">
-      <c r="A97">
+      <c r="A97" s="1">
         <v>96.000000</v>
       </c>
-      <c r="B97">
+      <c r="B97" s="1">
         <v>97.000000</v>
       </c>
-      <c r="C97">
+      <c r="C97" s="1">
         <f>A97+B97</f>
       </c>
     </row>
     <row r="98">
-      <c r="A98">
+      <c r="A98" s="1">
         <v>97.000000</v>
       </c>
-      <c r="B98">
+      <c r="B98" s="1">
         <v>98.000000</v>
       </c>
-      <c r="C98">
+      <c r="C98" s="1">
         <f>A98+B98</f>
       </c>
     </row>
     <row r="99">
-      <c r="A99">
+      <c r="A99" s="1">
         <v>98.000000</v>
       </c>
-      <c r="B99">
+      <c r="B99" s="1">
         <v>99.000000</v>
       </c>
-      <c r="C99">
+      <c r="C99" s="1">
         <f>A99+B99</f>
       </c>
     </row>
     <row r="100">
-      <c r="A100">
+      <c r="A100" s="1">
         <v>99.000000</v>
       </c>
-      <c r="B100">
+      <c r="B100" s="1">
         <v>100.000000</v>
       </c>
-      <c r="C100">
+      <c r="C100" s="1">
         <f>A100+B100</f>
       </c>
     </row>
     <row r="101">
-      <c r="A101">
+      <c r="A101" s="1">
         <v>100.000000</v>
       </c>
-      <c r="B101">
+      <c r="B101" s="1">
         <v>101.000000</v>
       </c>
-      <c r="C101">
+      <c r="C101" s="1">
         <f>A101+B101</f>
       </c>
     </row>
     <row r="102">
-      <c r="B102" s="52" t="inlineStr">
+      <c r="A102" s="2" t="inlineStr">
         <is>
           <t>total:</t>
         </is>
       </c>
-      <c r="C102">
+      <c r="B102" s="2"/>
+      <c r="C102" s="1">
         <f>SUM(C2:C101)</f>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A102:B102"/>
+  </mergeCells>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding custom row heights.
Adding custom row heights.
Using braces after if/else/else if; it's probably good practice.
Updated README.
</commit_message>
<xml_diff>
--- a/BasicWorkbook/test1.xlsx
+++ b/BasicWorkbook/test1.xlsx
@@ -98,7 +98,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" wrapText="false"/>
     </xf>
@@ -127,59 +130,77 @@
     <col min="1" max="1" width="9.005" bestFit="1"/>
     <col min="2" max="2" width="9.005" bestFit="1"/>
     <col min="3" max="3" width="9.005" bestFit="1"/>
+    <col min="4" max="4" width="9.005" bestFit="1"/>
+    <col min="5" max="5" width="9.005" bestFit="1"/>
+    <col min="6" max="6" width="9.005" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="68.000000" customHeight="1">
       <c r="A1" s="0" t="inlineStr">
+        <is>
+          <t>This workbook demonstrates some of the features of BasicWorkbook. For example, this cell demonstrates wrapped text in a merged cell with top left alignment and a custom row height.</t>
+        </is>
+      </c>
+      <c r="B1" s="0"/>
+      <c r="C1" s="0"/>
+      <c r="D1" s="0"/>
+      <c r="E1" s="0"/>
+      <c r="F1" s="0"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
         <is>
           <t>col 1</t>
         </is>
       </c>
-      <c r="B1" s="0" t="inlineStr">
+      <c r="B2" s="1" t="inlineStr">
         <is>
           <t>col 2</t>
         </is>
       </c>
-      <c r="C1" s="0" t="inlineStr">
+      <c r="C2" s="1" t="inlineStr">
         <is>
           <t>col 3</t>
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="1">
+    <row r="3">
+      <c r="A3" s="2">
         <v>1.000000</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B3" s="2">
         <v>4.000000</v>
       </c>
-      <c r="C2" s="1">
-        <f>A2+B2</f>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1">
+      <c r="C3" s="2">
+        <f>A3+B3</f>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2">
         <v>2.000000</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B4" s="2">
         <v>5.000000</v>
       </c>
-      <c r="C3" s="1">
-        <f>A3+B3</f>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1">
+      <c r="C4" s="2">
+        <f>A4+B4</f>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2">
         <v>3.000000</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B5" s="2">
         <v>6.000000</v>
       </c>
-      <c r="C4" s="1">
-        <f>A4+B4</f>
+      <c r="C5" s="2">
+        <f>A5+B5</f>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
 </worksheet>
 </file>
 
@@ -196,1130 +217,1130 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="0" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>col 1</t>
         </is>
       </c>
-      <c r="B1" s="0" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>col 2</t>
         </is>
       </c>
-      <c r="C1" s="0" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>col 3</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1">
+      <c r="A2" s="2">
         <v>1.000000</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
         <v>2.000000</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="2">
         <f>A2+B2</f>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1">
+      <c r="A3" s="2">
         <v>2.000000</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="2">
         <v>3.000000</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="2">
         <f>A3+B3</f>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1">
+      <c r="A4" s="2">
         <v>3.000000</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="2">
         <v>4.000000</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="2">
         <f>A4+B4</f>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1">
+      <c r="A5" s="2">
         <v>4.000000</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="2">
         <v>5.000000</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="2">
         <f>A5+B5</f>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1">
+      <c r="A6" s="2">
         <v>5.000000</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="2">
         <v>6.000000</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="2">
         <f>A6+B6</f>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1">
+      <c r="A7" s="2">
         <v>6.000000</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="2">
         <v>7.000000</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="2">
         <f>A7+B7</f>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1">
+      <c r="A8" s="2">
         <v>7.000000</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="2">
         <v>8.000000</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="2">
         <f>A8+B8</f>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1">
+      <c r="A9" s="2">
         <v>8.000000</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="2">
         <v>9.000000</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="2">
         <f>A9+B9</f>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1">
+      <c r="A10" s="2">
         <v>9.000000</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="2">
         <v>10.000000</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="2">
         <f>A10+B10</f>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1">
+      <c r="A11" s="2">
         <v>10.000000</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="2">
         <v>11.000000</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="2">
         <f>A11+B11</f>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1">
+      <c r="A12" s="2">
         <v>11.000000</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="2">
         <v>12.000000</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="2">
         <f>A12+B12</f>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1">
+      <c r="A13" s="2">
         <v>12.000000</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="2">
         <v>13.000000</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="2">
         <f>A13+B13</f>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1">
+      <c r="A14" s="2">
         <v>13.000000</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="2">
         <v>14.000000</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="2">
         <f>A14+B14</f>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="1">
+      <c r="A15" s="2">
         <v>14.000000</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="2">
         <v>15.000000</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="2">
         <f>A15+B15</f>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1">
+      <c r="A16" s="2">
         <v>15.000000</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="2">
         <v>16.000000</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="2">
         <f>A16+B16</f>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1">
+      <c r="A17" s="2">
         <v>16.000000</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="2">
         <v>17.000000</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="2">
         <f>A17+B17</f>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="1">
+      <c r="A18" s="2">
         <v>17.000000</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="2">
         <v>18.000000</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="2">
         <f>A18+B18</f>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="1">
+      <c r="A19" s="2">
         <v>18.000000</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="2">
         <v>19.000000</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="2">
         <f>A19+B19</f>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="1">
+      <c r="A20" s="2">
         <v>19.000000</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="2">
         <v>20.000000</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="2">
         <f>A20+B20</f>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="1">
+      <c r="A21" s="2">
         <v>20.000000</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="2">
         <v>21.000000</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" s="2">
         <f>A21+B21</f>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="1">
+      <c r="A22" s="2">
         <v>21.000000</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="2">
         <v>22.000000</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22" s="2">
         <f>A22+B22</f>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="1">
+      <c r="A23" s="2">
         <v>22.000000</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" s="2">
         <v>23.000000</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23" s="2">
         <f>A23+B23</f>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="1">
+      <c r="A24" s="2">
         <v>23.000000</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B24" s="2">
         <v>24.000000</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="2">
         <f>A24+B24</f>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="1">
+      <c r="A25" s="2">
         <v>24.000000</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="2">
         <v>25.000000</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25" s="2">
         <f>A25+B25</f>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="1">
+      <c r="A26" s="2">
         <v>25.000000</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26" s="2">
         <v>26.000000</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="2">
         <f>A26+B26</f>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="1">
+      <c r="A27" s="2">
         <v>26.000000</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B27" s="2">
         <v>27.000000</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27" s="2">
         <f>A27+B27</f>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="1">
+      <c r="A28" s="2">
         <v>27.000000</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="2">
         <v>28.000000</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28" s="2">
         <f>A28+B28</f>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="1">
+      <c r="A29" s="2">
         <v>28.000000</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29" s="2">
         <v>29.000000</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C29" s="2">
         <f>A29+B29</f>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="1">
+      <c r="A30" s="2">
         <v>29.000000</v>
       </c>
-      <c r="B30" s="1">
+      <c r="B30" s="2">
         <v>30.000000</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30" s="2">
         <f>A30+B30</f>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="1">
+      <c r="A31" s="2">
         <v>30.000000</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B31" s="2">
         <v>31.000000</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C31" s="2">
         <f>A31+B31</f>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="1">
+      <c r="A32" s="2">
         <v>31.000000</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B32" s="2">
         <v>32.000000</v>
       </c>
-      <c r="C32" s="1">
+      <c r="C32" s="2">
         <f>A32+B32</f>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="1">
+      <c r="A33" s="2">
         <v>32.000000</v>
       </c>
-      <c r="B33" s="1">
+      <c r="B33" s="2">
         <v>33.000000</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C33" s="2">
         <f>A33+B33</f>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="1">
+      <c r="A34" s="2">
         <v>33.000000</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B34" s="2">
         <v>34.000000</v>
       </c>
-      <c r="C34" s="1">
+      <c r="C34" s="2">
         <f>A34+B34</f>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="1">
+      <c r="A35" s="2">
         <v>34.000000</v>
       </c>
-      <c r="B35" s="1">
+      <c r="B35" s="2">
         <v>35.000000</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C35" s="2">
         <f>A35+B35</f>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="1">
+      <c r="A36" s="2">
         <v>35.000000</v>
       </c>
-      <c r="B36" s="1">
+      <c r="B36" s="2">
         <v>36.000000</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C36" s="2">
         <f>A36+B36</f>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="1">
+      <c r="A37" s="2">
         <v>36.000000</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B37" s="2">
         <v>37.000000</v>
       </c>
-      <c r="C37" s="1">
+      <c r="C37" s="2">
         <f>A37+B37</f>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="1">
+      <c r="A38" s="2">
         <v>37.000000</v>
       </c>
-      <c r="B38" s="1">
+      <c r="B38" s="2">
         <v>38.000000</v>
       </c>
-      <c r="C38" s="1">
+      <c r="C38" s="2">
         <f>A38+B38</f>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="1">
+      <c r="A39" s="2">
         <v>38.000000</v>
       </c>
-      <c r="B39" s="1">
+      <c r="B39" s="2">
         <v>39.000000</v>
       </c>
-      <c r="C39" s="1">
+      <c r="C39" s="2">
         <f>A39+B39</f>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="1">
+      <c r="A40" s="2">
         <v>39.000000</v>
       </c>
-      <c r="B40" s="1">
+      <c r="B40" s="2">
         <v>40.000000</v>
       </c>
-      <c r="C40" s="1">
+      <c r="C40" s="2">
         <f>A40+B40</f>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="1">
+      <c r="A41" s="2">
         <v>40.000000</v>
       </c>
-      <c r="B41" s="1">
+      <c r="B41" s="2">
         <v>41.000000</v>
       </c>
-      <c r="C41" s="1">
+      <c r="C41" s="2">
         <f>A41+B41</f>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="1">
+      <c r="A42" s="2">
         <v>41.000000</v>
       </c>
-      <c r="B42" s="1">
+      <c r="B42" s="2">
         <v>42.000000</v>
       </c>
-      <c r="C42" s="1">
+      <c r="C42" s="2">
         <f>A42+B42</f>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="1">
+      <c r="A43" s="2">
         <v>42.000000</v>
       </c>
-      <c r="B43" s="1">
+      <c r="B43" s="2">
         <v>43.000000</v>
       </c>
-      <c r="C43" s="1">
+      <c r="C43" s="2">
         <f>A43+B43</f>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="1">
+      <c r="A44" s="2">
         <v>43.000000</v>
       </c>
-      <c r="B44" s="1">
+      <c r="B44" s="2">
         <v>44.000000</v>
       </c>
-      <c r="C44" s="1">
+      <c r="C44" s="2">
         <f>A44+B44</f>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="1">
+      <c r="A45" s="2">
         <v>44.000000</v>
       </c>
-      <c r="B45" s="1">
+      <c r="B45" s="2">
         <v>45.000000</v>
       </c>
-      <c r="C45" s="1">
+      <c r="C45" s="2">
         <f>A45+B45</f>
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="1">
+      <c r="A46" s="2">
         <v>45.000000</v>
       </c>
-      <c r="B46" s="1">
+      <c r="B46" s="2">
         <v>46.000000</v>
       </c>
-      <c r="C46" s="1">
+      <c r="C46" s="2">
         <f>A46+B46</f>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="1">
+      <c r="A47" s="2">
         <v>46.000000</v>
       </c>
-      <c r="B47" s="1">
+      <c r="B47" s="2">
         <v>47.000000</v>
       </c>
-      <c r="C47" s="1">
+      <c r="C47" s="2">
         <f>A47+B47</f>
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="1">
+      <c r="A48" s="2">
         <v>47.000000</v>
       </c>
-      <c r="B48" s="1">
+      <c r="B48" s="2">
         <v>48.000000</v>
       </c>
-      <c r="C48" s="1">
+      <c r="C48" s="2">
         <f>A48+B48</f>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="1">
+      <c r="A49" s="2">
         <v>48.000000</v>
       </c>
-      <c r="B49" s="1">
+      <c r="B49" s="2">
         <v>49.000000</v>
       </c>
-      <c r="C49" s="1">
+      <c r="C49" s="2">
         <f>A49+B49</f>
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="1">
+      <c r="A50" s="2">
         <v>49.000000</v>
       </c>
-      <c r="B50" s="1">
+      <c r="B50" s="2">
         <v>50.000000</v>
       </c>
-      <c r="C50" s="1">
+      <c r="C50" s="2">
         <f>A50+B50</f>
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="1">
+      <c r="A51" s="2">
         <v>50.000000</v>
       </c>
-      <c r="B51" s="1">
+      <c r="B51" s="2">
         <v>51.000000</v>
       </c>
-      <c r="C51" s="1">
+      <c r="C51" s="2">
         <f>A51+B51</f>
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="1">
+      <c r="A52" s="2">
         <v>51.000000</v>
       </c>
-      <c r="B52" s="1">
+      <c r="B52" s="2">
         <v>52.000000</v>
       </c>
-      <c r="C52" s="1">
+      <c r="C52" s="2">
         <f>A52+B52</f>
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="1">
+      <c r="A53" s="2">
         <v>52.000000</v>
       </c>
-      <c r="B53" s="1">
+      <c r="B53" s="2">
         <v>53.000000</v>
       </c>
-      <c r="C53" s="1">
+      <c r="C53" s="2">
         <f>A53+B53</f>
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="1">
+      <c r="A54" s="2">
         <v>53.000000</v>
       </c>
-      <c r="B54" s="1">
+      <c r="B54" s="2">
         <v>54.000000</v>
       </c>
-      <c r="C54" s="1">
+      <c r="C54" s="2">
         <f>A54+B54</f>
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="1">
+      <c r="A55" s="2">
         <v>54.000000</v>
       </c>
-      <c r="B55" s="1">
+      <c r="B55" s="2">
         <v>55.000000</v>
       </c>
-      <c r="C55" s="1">
+      <c r="C55" s="2">
         <f>A55+B55</f>
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="1">
+      <c r="A56" s="2">
         <v>55.000000</v>
       </c>
-      <c r="B56" s="1">
+      <c r="B56" s="2">
         <v>56.000000</v>
       </c>
-      <c r="C56" s="1">
+      <c r="C56" s="2">
         <f>A56+B56</f>
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="1">
+      <c r="A57" s="2">
         <v>56.000000</v>
       </c>
-      <c r="B57" s="1">
+      <c r="B57" s="2">
         <v>57.000000</v>
       </c>
-      <c r="C57" s="1">
+      <c r="C57" s="2">
         <f>A57+B57</f>
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="1">
+      <c r="A58" s="2">
         <v>57.000000</v>
       </c>
-      <c r="B58" s="1">
+      <c r="B58" s="2">
         <v>58.000000</v>
       </c>
-      <c r="C58" s="1">
+      <c r="C58" s="2">
         <f>A58+B58</f>
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="1">
+      <c r="A59" s="2">
         <v>58.000000</v>
       </c>
-      <c r="B59" s="1">
+      <c r="B59" s="2">
         <v>59.000000</v>
       </c>
-      <c r="C59" s="1">
+      <c r="C59" s="2">
         <f>A59+B59</f>
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="1">
+      <c r="A60" s="2">
         <v>59.000000</v>
       </c>
-      <c r="B60" s="1">
+      <c r="B60" s="2">
         <v>60.000000</v>
       </c>
-      <c r="C60" s="1">
+      <c r="C60" s="2">
         <f>A60+B60</f>
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="1">
+      <c r="A61" s="2">
         <v>60.000000</v>
       </c>
-      <c r="B61" s="1">
+      <c r="B61" s="2">
         <v>61.000000</v>
       </c>
-      <c r="C61" s="1">
+      <c r="C61" s="2">
         <f>A61+B61</f>
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="1">
+      <c r="A62" s="2">
         <v>61.000000</v>
       </c>
-      <c r="B62" s="1">
+      <c r="B62" s="2">
         <v>62.000000</v>
       </c>
-      <c r="C62" s="1">
+      <c r="C62" s="2">
         <f>A62+B62</f>
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="1">
+      <c r="A63" s="2">
         <v>62.000000</v>
       </c>
-      <c r="B63" s="1">
+      <c r="B63" s="2">
         <v>63.000000</v>
       </c>
-      <c r="C63" s="1">
+      <c r="C63" s="2">
         <f>A63+B63</f>
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="1">
+      <c r="A64" s="2">
         <v>63.000000</v>
       </c>
-      <c r="B64" s="1">
+      <c r="B64" s="2">
         <v>64.000000</v>
       </c>
-      <c r="C64" s="1">
+      <c r="C64" s="2">
         <f>A64+B64</f>
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="1">
+      <c r="A65" s="2">
         <v>64.000000</v>
       </c>
-      <c r="B65" s="1">
+      <c r="B65" s="2">
         <v>65.000000</v>
       </c>
-      <c r="C65" s="1">
+      <c r="C65" s="2">
         <f>A65+B65</f>
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="1">
+      <c r="A66" s="2">
         <v>65.000000</v>
       </c>
-      <c r="B66" s="1">
+      <c r="B66" s="2">
         <v>66.000000</v>
       </c>
-      <c r="C66" s="1">
+      <c r="C66" s="2">
         <f>A66+B66</f>
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="1">
+      <c r="A67" s="2">
         <v>66.000000</v>
       </c>
-      <c r="B67" s="1">
+      <c r="B67" s="2">
         <v>67.000000</v>
       </c>
-      <c r="C67" s="1">
+      <c r="C67" s="2">
         <f>A67+B67</f>
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="1">
+      <c r="A68" s="2">
         <v>67.000000</v>
       </c>
-      <c r="B68" s="1">
+      <c r="B68" s="2">
         <v>68.000000</v>
       </c>
-      <c r="C68" s="1">
+      <c r="C68" s="2">
         <f>A68+B68</f>
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="1">
+      <c r="A69" s="2">
         <v>68.000000</v>
       </c>
-      <c r="B69" s="1">
+      <c r="B69" s="2">
         <v>69.000000</v>
       </c>
-      <c r="C69" s="1">
+      <c r="C69" s="2">
         <f>A69+B69</f>
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="1">
+      <c r="A70" s="2">
         <v>69.000000</v>
       </c>
-      <c r="B70" s="1">
+      <c r="B70" s="2">
         <v>70.000000</v>
       </c>
-      <c r="C70" s="1">
+      <c r="C70" s="2">
         <f>A70+B70</f>
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="1">
+      <c r="A71" s="2">
         <v>70.000000</v>
       </c>
-      <c r="B71" s="1">
+      <c r="B71" s="2">
         <v>71.000000</v>
       </c>
-      <c r="C71" s="1">
+      <c r="C71" s="2">
         <f>A71+B71</f>
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="1">
+      <c r="A72" s="2">
         <v>71.000000</v>
       </c>
-      <c r="B72" s="1">
+      <c r="B72" s="2">
         <v>72.000000</v>
       </c>
-      <c r="C72" s="1">
+      <c r="C72" s="2">
         <f>A72+B72</f>
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="1">
+      <c r="A73" s="2">
         <v>72.000000</v>
       </c>
-      <c r="B73" s="1">
+      <c r="B73" s="2">
         <v>73.000000</v>
       </c>
-      <c r="C73" s="1">
+      <c r="C73" s="2">
         <f>A73+B73</f>
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="1">
+      <c r="A74" s="2">
         <v>73.000000</v>
       </c>
-      <c r="B74" s="1">
+      <c r="B74" s="2">
         <v>74.000000</v>
       </c>
-      <c r="C74" s="1">
+      <c r="C74" s="2">
         <f>A74+B74</f>
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="1">
+      <c r="A75" s="2">
         <v>74.000000</v>
       </c>
-      <c r="B75" s="1">
+      <c r="B75" s="2">
         <v>75.000000</v>
       </c>
-      <c r="C75" s="1">
+      <c r="C75" s="2">
         <f>A75+B75</f>
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="1">
+      <c r="A76" s="2">
         <v>75.000000</v>
       </c>
-      <c r="B76" s="1">
+      <c r="B76" s="2">
         <v>76.000000</v>
       </c>
-      <c r="C76" s="1">
+      <c r="C76" s="2">
         <f>A76+B76</f>
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="1">
+      <c r="A77" s="2">
         <v>76.000000</v>
       </c>
-      <c r="B77" s="1">
+      <c r="B77" s="2">
         <v>77.000000</v>
       </c>
-      <c r="C77" s="1">
+      <c r="C77" s="2">
         <f>A77+B77</f>
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="1">
+      <c r="A78" s="2">
         <v>77.000000</v>
       </c>
-      <c r="B78" s="1">
+      <c r="B78" s="2">
         <v>78.000000</v>
       </c>
-      <c r="C78" s="1">
+      <c r="C78" s="2">
         <f>A78+B78</f>
       </c>
     </row>
     <row r="79">
-      <c r="A79" s="1">
+      <c r="A79" s="2">
         <v>78.000000</v>
       </c>
-      <c r="B79" s="1">
+      <c r="B79" s="2">
         <v>79.000000</v>
       </c>
-      <c r="C79" s="1">
+      <c r="C79" s="2">
         <f>A79+B79</f>
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="1">
+      <c r="A80" s="2">
         <v>79.000000</v>
       </c>
-      <c r="B80" s="1">
+      <c r="B80" s="2">
         <v>80.000000</v>
       </c>
-      <c r="C80" s="1">
+      <c r="C80" s="2">
         <f>A80+B80</f>
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="1">
+      <c r="A81" s="2">
         <v>80.000000</v>
       </c>
-      <c r="B81" s="1">
+      <c r="B81" s="2">
         <v>81.000000</v>
       </c>
-      <c r="C81" s="1">
+      <c r="C81" s="2">
         <f>A81+B81</f>
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="1">
+      <c r="A82" s="2">
         <v>81.000000</v>
       </c>
-      <c r="B82" s="1">
+      <c r="B82" s="2">
         <v>82.000000</v>
       </c>
-      <c r="C82" s="1">
+      <c r="C82" s="2">
         <f>A82+B82</f>
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="1">
+      <c r="A83" s="2">
         <v>82.000000</v>
       </c>
-      <c r="B83" s="1">
+      <c r="B83" s="2">
         <v>83.000000</v>
       </c>
-      <c r="C83" s="1">
+      <c r="C83" s="2">
         <f>A83+B83</f>
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="1">
+      <c r="A84" s="2">
         <v>83.000000</v>
       </c>
-      <c r="B84" s="1">
+      <c r="B84" s="2">
         <v>84.000000</v>
       </c>
-      <c r="C84" s="1">
+      <c r="C84" s="2">
         <f>A84+B84</f>
       </c>
     </row>
     <row r="85">
-      <c r="A85" s="1">
+      <c r="A85" s="2">
         <v>84.000000</v>
       </c>
-      <c r="B85" s="1">
+      <c r="B85" s="2">
         <v>85.000000</v>
       </c>
-      <c r="C85" s="1">
+      <c r="C85" s="2">
         <f>A85+B85</f>
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="1">
+      <c r="A86" s="2">
         <v>85.000000</v>
       </c>
-      <c r="B86" s="1">
+      <c r="B86" s="2">
         <v>86.000000</v>
       </c>
-      <c r="C86" s="1">
+      <c r="C86" s="2">
         <f>A86+B86</f>
       </c>
     </row>
     <row r="87">
-      <c r="A87" s="1">
+      <c r="A87" s="2">
         <v>86.000000</v>
       </c>
-      <c r="B87" s="1">
+      <c r="B87" s="2">
         <v>87.000000</v>
       </c>
-      <c r="C87" s="1">
+      <c r="C87" s="2">
         <f>A87+B87</f>
       </c>
     </row>
     <row r="88">
-      <c r="A88" s="1">
+      <c r="A88" s="2">
         <v>87.000000</v>
       </c>
-      <c r="B88" s="1">
+      <c r="B88" s="2">
         <v>88.000000</v>
       </c>
-      <c r="C88" s="1">
+      <c r="C88" s="2">
         <f>A88+B88</f>
       </c>
     </row>
     <row r="89">
-      <c r="A89" s="1">
+      <c r="A89" s="2">
         <v>88.000000</v>
       </c>
-      <c r="B89" s="1">
+      <c r="B89" s="2">
         <v>89.000000</v>
       </c>
-      <c r="C89" s="1">
+      <c r="C89" s="2">
         <f>A89+B89</f>
       </c>
     </row>
     <row r="90">
-      <c r="A90" s="1">
+      <c r="A90" s="2">
         <v>89.000000</v>
       </c>
-      <c r="B90" s="1">
+      <c r="B90" s="2">
         <v>90.000000</v>
       </c>
-      <c r="C90" s="1">
+      <c r="C90" s="2">
         <f>A90+B90</f>
       </c>
     </row>
     <row r="91">
-      <c r="A91" s="1">
+      <c r="A91" s="2">
         <v>90.000000</v>
       </c>
-      <c r="B91" s="1">
+      <c r="B91" s="2">
         <v>91.000000</v>
       </c>
-      <c r="C91" s="1">
+      <c r="C91" s="2">
         <f>A91+B91</f>
       </c>
     </row>
     <row r="92">
-      <c r="A92" s="1">
+      <c r="A92" s="2">
         <v>91.000000</v>
       </c>
-      <c r="B92" s="1">
+      <c r="B92" s="2">
         <v>92.000000</v>
       </c>
-      <c r="C92" s="1">
+      <c r="C92" s="2">
         <f>A92+B92</f>
       </c>
     </row>
     <row r="93">
-      <c r="A93" s="1">
+      <c r="A93" s="2">
         <v>92.000000</v>
       </c>
-      <c r="B93" s="1">
+      <c r="B93" s="2">
         <v>93.000000</v>
       </c>
-      <c r="C93" s="1">
+      <c r="C93" s="2">
         <f>A93+B93</f>
       </c>
     </row>
     <row r="94">
-      <c r="A94" s="1">
+      <c r="A94" s="2">
         <v>93.000000</v>
       </c>
-      <c r="B94" s="1">
+      <c r="B94" s="2">
         <v>94.000000</v>
       </c>
-      <c r="C94" s="1">
+      <c r="C94" s="2">
         <f>A94+B94</f>
       </c>
     </row>
     <row r="95">
-      <c r="A95" s="1">
+      <c r="A95" s="2">
         <v>94.000000</v>
       </c>
-      <c r="B95" s="1">
+      <c r="B95" s="2">
         <v>95.000000</v>
       </c>
-      <c r="C95" s="1">
+      <c r="C95" s="2">
         <f>A95+B95</f>
       </c>
     </row>
     <row r="96">
-      <c r="A96" s="1">
+      <c r="A96" s="2">
         <v>95.000000</v>
       </c>
-      <c r="B96" s="1">
+      <c r="B96" s="2">
         <v>96.000000</v>
       </c>
-      <c r="C96" s="1">
+      <c r="C96" s="2">
         <f>A96+B96</f>
       </c>
     </row>
     <row r="97">
-      <c r="A97" s="1">
+      <c r="A97" s="2">
         <v>96.000000</v>
       </c>
-      <c r="B97" s="1">
+      <c r="B97" s="2">
         <v>97.000000</v>
       </c>
-      <c r="C97" s="1">
+      <c r="C97" s="2">
         <f>A97+B97</f>
       </c>
     </row>
     <row r="98">
-      <c r="A98" s="1">
+      <c r="A98" s="2">
         <v>97.000000</v>
       </c>
-      <c r="B98" s="1">
+      <c r="B98" s="2">
         <v>98.000000</v>
       </c>
-      <c r="C98" s="1">
+      <c r="C98" s="2">
         <f>A98+B98</f>
       </c>
     </row>
     <row r="99">
-      <c r="A99" s="1">
+      <c r="A99" s="2">
         <v>98.000000</v>
       </c>
-      <c r="B99" s="1">
+      <c r="B99" s="2">
         <v>99.000000</v>
       </c>
-      <c r="C99" s="1">
+      <c r="C99" s="2">
         <f>A99+B99</f>
       </c>
     </row>
     <row r="100">
-      <c r="A100" s="1">
+      <c r="A100" s="2">
         <v>99.000000</v>
       </c>
-      <c r="B100" s="1">
+      <c r="B100" s="2">
         <v>100.000000</v>
       </c>
-      <c r="C100" s="1">
+      <c r="C100" s="2">
         <f>A100+B100</f>
       </c>
     </row>
     <row r="101">
-      <c r="A101" s="1">
+      <c r="A101" s="2">
         <v>100.000000</v>
       </c>
-      <c r="B101" s="1">
+      <c r="B101" s="2">
         <v>101.000000</v>
       </c>
-      <c r="C101" s="1">
+      <c r="C101" s="2">
         <f>A101+B101</f>
       </c>
     </row>
     <row r="102">
-      <c r="A102" s="2" t="inlineStr">
+      <c r="A102" s="3" t="inlineStr">
         <is>
           <t>total:</t>
         </is>
       </c>
-      <c r="B102" s="2"/>
-      <c r="C102" s="1">
+      <c r="B102" s="3"/>
+      <c r="C102" s="2">
         <f>SUM(C2:C101)</f>
       </c>
     </row>

</xml_diff>

<commit_message>
Rebuilding demo, example output.
Rebuilding BasicWorkbookDemo.exe and example output after recent change.
</commit_message>
<xml_diff>
--- a/BasicWorkbook/test1.xlsx
+++ b/BasicWorkbook/test1.xlsx
@@ -99,14 +99,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="general" vertical="bottom" wrapText="false"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="true"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" wrapText="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" wrapText="false"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="bottom" wrapText="false"/>
@@ -136,64 +136,64 @@
   </cols>
   <sheetData>
     <row r="1" ht="68.000000" customHeight="1">
-      <c r="A1" s="0" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>This workbook demonstrates some of the features of BasicWorkbook. For example, this cell demonstrates wrapped text in a merged cell with top left alignment and a custom row height.</t>
         </is>
       </c>
-      <c r="B1" s="0"/>
-      <c r="C1" s="0"/>
-      <c r="D1" s="0"/>
-      <c r="E1" s="0"/>
-      <c r="F1" s="0"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
+      <c r="A2" s="2" t="inlineStr">
         <is>
           <t>col 1</t>
         </is>
       </c>
-      <c r="B2" s="1" t="inlineStr">
+      <c r="B2" s="2" t="inlineStr">
         <is>
           <t>col 2</t>
         </is>
       </c>
-      <c r="C2" s="1" t="inlineStr">
+      <c r="C2" s="2" t="inlineStr">
         <is>
           <t>col 3</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2">
+      <c r="A3" s="0">
         <v>1.000000</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="0">
         <v>4.000000</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="0">
         <f>A3+B3</f>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2">
+      <c r="A4" s="0">
         <v>2.000000</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="0">
         <v>5.000000</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="0">
         <f>A4+B4</f>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2">
+      <c r="A5" s="0">
         <v>3.000000</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="0">
         <v>6.000000</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="0">
         <f>A5+B5</f>
       </c>
     </row>
@@ -217,1119 +217,1119 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>col 1</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>col 2</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>col 3</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2">
+      <c r="A2" s="0">
         <v>1.000000</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="0">
         <v>2.000000</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="0">
         <f>A2+B2</f>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2">
+      <c r="A3" s="0">
         <v>2.000000</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="0">
         <v>3.000000</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="0">
         <f>A3+B3</f>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2">
+      <c r="A4" s="0">
         <v>3.000000</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="0">
         <v>4.000000</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="0">
         <f>A4+B4</f>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2">
+      <c r="A5" s="0">
         <v>4.000000</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="0">
         <v>5.000000</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="0">
         <f>A5+B5</f>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2">
+      <c r="A6" s="0">
         <v>5.000000</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="0">
         <v>6.000000</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="0">
         <f>A6+B6</f>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="2">
+      <c r="A7" s="0">
         <v>6.000000</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="0">
         <v>7.000000</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="0">
         <f>A7+B7</f>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="2">
+      <c r="A8" s="0">
         <v>7.000000</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="0">
         <v>8.000000</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="0">
         <f>A8+B8</f>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="2">
+      <c r="A9" s="0">
         <v>8.000000</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="0">
         <v>9.000000</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="0">
         <f>A9+B9</f>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="2">
+      <c r="A10" s="0">
         <v>9.000000</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="0">
         <v>10.000000</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="0">
         <f>A10+B10</f>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="2">
+      <c r="A11" s="0">
         <v>10.000000</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="0">
         <v>11.000000</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="0">
         <f>A11+B11</f>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="2">
+      <c r="A12" s="0">
         <v>11.000000</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="0">
         <v>12.000000</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="0">
         <f>A12+B12</f>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="2">
+      <c r="A13" s="0">
         <v>12.000000</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="0">
         <v>13.000000</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="0">
         <f>A13+B13</f>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="2">
+      <c r="A14" s="0">
         <v>13.000000</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="0">
         <v>14.000000</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="0">
         <f>A14+B14</f>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="2">
+      <c r="A15" s="0">
         <v>14.000000</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="0">
         <v>15.000000</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="0">
         <f>A15+B15</f>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="2">
+      <c r="A16" s="0">
         <v>15.000000</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="0">
         <v>16.000000</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="0">
         <f>A16+B16</f>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="2">
+      <c r="A17" s="0">
         <v>16.000000</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="0">
         <v>17.000000</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="0">
         <f>A17+B17</f>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="2">
+      <c r="A18" s="0">
         <v>17.000000</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="0">
         <v>18.000000</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="0">
         <f>A18+B18</f>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="2">
+      <c r="A19" s="0">
         <v>18.000000</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="0">
         <v>19.000000</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="0">
         <f>A19+B19</f>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="2">
+      <c r="A20" s="0">
         <v>19.000000</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="0">
         <v>20.000000</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="0">
         <f>A20+B20</f>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="2">
+      <c r="A21" s="0">
         <v>20.000000</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="0">
         <v>21.000000</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="0">
         <f>A21+B21</f>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="2">
+      <c r="A22" s="0">
         <v>21.000000</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="0">
         <v>22.000000</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="0">
         <f>A22+B22</f>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="2">
+      <c r="A23" s="0">
         <v>22.000000</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="0">
         <v>23.000000</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="0">
         <f>A23+B23</f>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="2">
+      <c r="A24" s="0">
         <v>23.000000</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24" s="0">
         <v>24.000000</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="0">
         <f>A24+B24</f>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="2">
+      <c r="A25" s="0">
         <v>24.000000</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25" s="0">
         <v>25.000000</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="0">
         <f>A25+B25</f>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="2">
+      <c r="A26" s="0">
         <v>25.000000</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B26" s="0">
         <v>26.000000</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="0">
         <f>A26+B26</f>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="2">
+      <c r="A27" s="0">
         <v>26.000000</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B27" s="0">
         <v>27.000000</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="0">
         <f>A27+B27</f>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="2">
+      <c r="A28" s="0">
         <v>27.000000</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B28" s="0">
         <v>28.000000</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="0">
         <f>A28+B28</f>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="2">
+      <c r="A29" s="0">
         <v>28.000000</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B29" s="0">
         <v>29.000000</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="0">
         <f>A29+B29</f>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="2">
+      <c r="A30" s="0">
         <v>29.000000</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B30" s="0">
         <v>30.000000</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30" s="0">
         <f>A30+B30</f>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="2">
+      <c r="A31" s="0">
         <v>30.000000</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B31" s="0">
         <v>31.000000</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31" s="0">
         <f>A31+B31</f>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="2">
+      <c r="A32" s="0">
         <v>31.000000</v>
       </c>
-      <c r="B32" s="2">
+      <c r="B32" s="0">
         <v>32.000000</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32" s="0">
         <f>A32+B32</f>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="2">
+      <c r="A33" s="0">
         <v>32.000000</v>
       </c>
-      <c r="B33" s="2">
+      <c r="B33" s="0">
         <v>33.000000</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33" s="0">
         <f>A33+B33</f>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="2">
+      <c r="A34" s="0">
         <v>33.000000</v>
       </c>
-      <c r="B34" s="2">
+      <c r="B34" s="0">
         <v>34.000000</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C34" s="0">
         <f>A34+B34</f>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="2">
+      <c r="A35" s="0">
         <v>34.000000</v>
       </c>
-      <c r="B35" s="2">
+      <c r="B35" s="0">
         <v>35.000000</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C35" s="0">
         <f>A35+B35</f>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="2">
+      <c r="A36" s="0">
         <v>35.000000</v>
       </c>
-      <c r="B36" s="2">
+      <c r="B36" s="0">
         <v>36.000000</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C36" s="0">
         <f>A36+B36</f>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="2">
+      <c r="A37" s="0">
         <v>36.000000</v>
       </c>
-      <c r="B37" s="2">
+      <c r="B37" s="0">
         <v>37.000000</v>
       </c>
-      <c r="C37" s="2">
+      <c r="C37" s="0">
         <f>A37+B37</f>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="2">
+      <c r="A38" s="0">
         <v>37.000000</v>
       </c>
-      <c r="B38" s="2">
+      <c r="B38" s="0">
         <v>38.000000</v>
       </c>
-      <c r="C38" s="2">
+      <c r="C38" s="0">
         <f>A38+B38</f>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="2">
+      <c r="A39" s="0">
         <v>38.000000</v>
       </c>
-      <c r="B39" s="2">
+      <c r="B39" s="0">
         <v>39.000000</v>
       </c>
-      <c r="C39" s="2">
+      <c r="C39" s="0">
         <f>A39+B39</f>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="2">
+      <c r="A40" s="0">
         <v>39.000000</v>
       </c>
-      <c r="B40" s="2">
+      <c r="B40" s="0">
         <v>40.000000</v>
       </c>
-      <c r="C40" s="2">
+      <c r="C40" s="0">
         <f>A40+B40</f>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="2">
+      <c r="A41" s="0">
         <v>40.000000</v>
       </c>
-      <c r="B41" s="2">
+      <c r="B41" s="0">
         <v>41.000000</v>
       </c>
-      <c r="C41" s="2">
+      <c r="C41" s="0">
         <f>A41+B41</f>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="2">
+      <c r="A42" s="0">
         <v>41.000000</v>
       </c>
-      <c r="B42" s="2">
+      <c r="B42" s="0">
         <v>42.000000</v>
       </c>
-      <c r="C42" s="2">
+      <c r="C42" s="0">
         <f>A42+B42</f>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="2">
+      <c r="A43" s="0">
         <v>42.000000</v>
       </c>
-      <c r="B43" s="2">
+      <c r="B43" s="0">
         <v>43.000000</v>
       </c>
-      <c r="C43" s="2">
+      <c r="C43" s="0">
         <f>A43+B43</f>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="2">
+      <c r="A44" s="0">
         <v>43.000000</v>
       </c>
-      <c r="B44" s="2">
+      <c r="B44" s="0">
         <v>44.000000</v>
       </c>
-      <c r="C44" s="2">
+      <c r="C44" s="0">
         <f>A44+B44</f>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="2">
+      <c r="A45" s="0">
         <v>44.000000</v>
       </c>
-      <c r="B45" s="2">
+      <c r="B45" s="0">
         <v>45.000000</v>
       </c>
-      <c r="C45" s="2">
+      <c r="C45" s="0">
         <f>A45+B45</f>
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="2">
+      <c r="A46" s="0">
         <v>45.000000</v>
       </c>
-      <c r="B46" s="2">
+      <c r="B46" s="0">
         <v>46.000000</v>
       </c>
-      <c r="C46" s="2">
+      <c r="C46" s="0">
         <f>A46+B46</f>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="2">
+      <c r="A47" s="0">
         <v>46.000000</v>
       </c>
-      <c r="B47" s="2">
+      <c r="B47" s="0">
         <v>47.000000</v>
       </c>
-      <c r="C47" s="2">
+      <c r="C47" s="0">
         <f>A47+B47</f>
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="2">
+      <c r="A48" s="0">
         <v>47.000000</v>
       </c>
-      <c r="B48" s="2">
+      <c r="B48" s="0">
         <v>48.000000</v>
       </c>
-      <c r="C48" s="2">
+      <c r="C48" s="0">
         <f>A48+B48</f>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="2">
+      <c r="A49" s="0">
         <v>48.000000</v>
       </c>
-      <c r="B49" s="2">
+      <c r="B49" s="0">
         <v>49.000000</v>
       </c>
-      <c r="C49" s="2">
+      <c r="C49" s="0">
         <f>A49+B49</f>
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="2">
+      <c r="A50" s="0">
         <v>49.000000</v>
       </c>
-      <c r="B50" s="2">
+      <c r="B50" s="0">
         <v>50.000000</v>
       </c>
-      <c r="C50" s="2">
+      <c r="C50" s="0">
         <f>A50+B50</f>
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="2">
+      <c r="A51" s="0">
         <v>50.000000</v>
       </c>
-      <c r="B51" s="2">
+      <c r="B51" s="0">
         <v>51.000000</v>
       </c>
-      <c r="C51" s="2">
+      <c r="C51" s="0">
         <f>A51+B51</f>
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="2">
+      <c r="A52" s="0">
         <v>51.000000</v>
       </c>
-      <c r="B52" s="2">
+      <c r="B52" s="0">
         <v>52.000000</v>
       </c>
-      <c r="C52" s="2">
+      <c r="C52" s="0">
         <f>A52+B52</f>
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="2">
+      <c r="A53" s="0">
         <v>52.000000</v>
       </c>
-      <c r="B53" s="2">
+      <c r="B53" s="0">
         <v>53.000000</v>
       </c>
-      <c r="C53" s="2">
+      <c r="C53" s="0">
         <f>A53+B53</f>
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="2">
+      <c r="A54" s="0">
         <v>53.000000</v>
       </c>
-      <c r="B54" s="2">
+      <c r="B54" s="0">
         <v>54.000000</v>
       </c>
-      <c r="C54" s="2">
+      <c r="C54" s="0">
         <f>A54+B54</f>
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="2">
+      <c r="A55" s="0">
         <v>54.000000</v>
       </c>
-      <c r="B55" s="2">
+      <c r="B55" s="0">
         <v>55.000000</v>
       </c>
-      <c r="C55" s="2">
+      <c r="C55" s="0">
         <f>A55+B55</f>
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="2">
+      <c r="A56" s="0">
         <v>55.000000</v>
       </c>
-      <c r="B56" s="2">
+      <c r="B56" s="0">
         <v>56.000000</v>
       </c>
-      <c r="C56" s="2">
+      <c r="C56" s="0">
         <f>A56+B56</f>
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="2">
+      <c r="A57" s="0">
         <v>56.000000</v>
       </c>
-      <c r="B57" s="2">
+      <c r="B57" s="0">
         <v>57.000000</v>
       </c>
-      <c r="C57" s="2">
+      <c r="C57" s="0">
         <f>A57+B57</f>
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="2">
+      <c r="A58" s="0">
         <v>57.000000</v>
       </c>
-      <c r="B58" s="2">
+      <c r="B58" s="0">
         <v>58.000000</v>
       </c>
-      <c r="C58" s="2">
+      <c r="C58" s="0">
         <f>A58+B58</f>
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="2">
+      <c r="A59" s="0">
         <v>58.000000</v>
       </c>
-      <c r="B59" s="2">
+      <c r="B59" s="0">
         <v>59.000000</v>
       </c>
-      <c r="C59" s="2">
+      <c r="C59" s="0">
         <f>A59+B59</f>
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="2">
+      <c r="A60" s="0">
         <v>59.000000</v>
       </c>
-      <c r="B60" s="2">
+      <c r="B60" s="0">
         <v>60.000000</v>
       </c>
-      <c r="C60" s="2">
+      <c r="C60" s="0">
         <f>A60+B60</f>
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="2">
+      <c r="A61" s="0">
         <v>60.000000</v>
       </c>
-      <c r="B61" s="2">
+      <c r="B61" s="0">
         <v>61.000000</v>
       </c>
-      <c r="C61" s="2">
+      <c r="C61" s="0">
         <f>A61+B61</f>
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="2">
+      <c r="A62" s="0">
         <v>61.000000</v>
       </c>
-      <c r="B62" s="2">
+      <c r="B62" s="0">
         <v>62.000000</v>
       </c>
-      <c r="C62" s="2">
+      <c r="C62" s="0">
         <f>A62+B62</f>
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="2">
+      <c r="A63" s="0">
         <v>62.000000</v>
       </c>
-      <c r="B63" s="2">
+      <c r="B63" s="0">
         <v>63.000000</v>
       </c>
-      <c r="C63" s="2">
+      <c r="C63" s="0">
         <f>A63+B63</f>
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="2">
+      <c r="A64" s="0">
         <v>63.000000</v>
       </c>
-      <c r="B64" s="2">
+      <c r="B64" s="0">
         <v>64.000000</v>
       </c>
-      <c r="C64" s="2">
+      <c r="C64" s="0">
         <f>A64+B64</f>
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="2">
+      <c r="A65" s="0">
         <v>64.000000</v>
       </c>
-      <c r="B65" s="2">
+      <c r="B65" s="0">
         <v>65.000000</v>
       </c>
-      <c r="C65" s="2">
+      <c r="C65" s="0">
         <f>A65+B65</f>
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="2">
+      <c r="A66" s="0">
         <v>65.000000</v>
       </c>
-      <c r="B66" s="2">
+      <c r="B66" s="0">
         <v>66.000000</v>
       </c>
-      <c r="C66" s="2">
+      <c r="C66" s="0">
         <f>A66+B66</f>
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="2">
+      <c r="A67" s="0">
         <v>66.000000</v>
       </c>
-      <c r="B67" s="2">
+      <c r="B67" s="0">
         <v>67.000000</v>
       </c>
-      <c r="C67" s="2">
+      <c r="C67" s="0">
         <f>A67+B67</f>
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="2">
+      <c r="A68" s="0">
         <v>67.000000</v>
       </c>
-      <c r="B68" s="2">
+      <c r="B68" s="0">
         <v>68.000000</v>
       </c>
-      <c r="C68" s="2">
+      <c r="C68" s="0">
         <f>A68+B68</f>
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="2">
+      <c r="A69" s="0">
         <v>68.000000</v>
       </c>
-      <c r="B69" s="2">
+      <c r="B69" s="0">
         <v>69.000000</v>
       </c>
-      <c r="C69" s="2">
+      <c r="C69" s="0">
         <f>A69+B69</f>
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="2">
+      <c r="A70" s="0">
         <v>69.000000</v>
       </c>
-      <c r="B70" s="2">
+      <c r="B70" s="0">
         <v>70.000000</v>
       </c>
-      <c r="C70" s="2">
+      <c r="C70" s="0">
         <f>A70+B70</f>
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="2">
+      <c r="A71" s="0">
         <v>70.000000</v>
       </c>
-      <c r="B71" s="2">
+      <c r="B71" s="0">
         <v>71.000000</v>
       </c>
-      <c r="C71" s="2">
+      <c r="C71" s="0">
         <f>A71+B71</f>
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="2">
+      <c r="A72" s="0">
         <v>71.000000</v>
       </c>
-      <c r="B72" s="2">
+      <c r="B72" s="0">
         <v>72.000000</v>
       </c>
-      <c r="C72" s="2">
+      <c r="C72" s="0">
         <f>A72+B72</f>
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="2">
+      <c r="A73" s="0">
         <v>72.000000</v>
       </c>
-      <c r="B73" s="2">
+      <c r="B73" s="0">
         <v>73.000000</v>
       </c>
-      <c r="C73" s="2">
+      <c r="C73" s="0">
         <f>A73+B73</f>
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="2">
+      <c r="A74" s="0">
         <v>73.000000</v>
       </c>
-      <c r="B74" s="2">
+      <c r="B74" s="0">
         <v>74.000000</v>
       </c>
-      <c r="C74" s="2">
+      <c r="C74" s="0">
         <f>A74+B74</f>
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="2">
+      <c r="A75" s="0">
         <v>74.000000</v>
       </c>
-      <c r="B75" s="2">
+      <c r="B75" s="0">
         <v>75.000000</v>
       </c>
-      <c r="C75" s="2">
+      <c r="C75" s="0">
         <f>A75+B75</f>
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="2">
+      <c r="A76" s="0">
         <v>75.000000</v>
       </c>
-      <c r="B76" s="2">
+      <c r="B76" s="0">
         <v>76.000000</v>
       </c>
-      <c r="C76" s="2">
+      <c r="C76" s="0">
         <f>A76+B76</f>
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="2">
+      <c r="A77" s="0">
         <v>76.000000</v>
       </c>
-      <c r="B77" s="2">
+      <c r="B77" s="0">
         <v>77.000000</v>
       </c>
-      <c r="C77" s="2">
+      <c r="C77" s="0">
         <f>A77+B77</f>
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="2">
+      <c r="A78" s="0">
         <v>77.000000</v>
       </c>
-      <c r="B78" s="2">
+      <c r="B78" s="0">
         <v>78.000000</v>
       </c>
-      <c r="C78" s="2">
+      <c r="C78" s="0">
         <f>A78+B78</f>
       </c>
     </row>
     <row r="79">
-      <c r="A79" s="2">
+      <c r="A79" s="0">
         <v>78.000000</v>
       </c>
-      <c r="B79" s="2">
+      <c r="B79" s="0">
         <v>79.000000</v>
       </c>
-      <c r="C79" s="2">
+      <c r="C79" s="0">
         <f>A79+B79</f>
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="2">
+      <c r="A80" s="0">
         <v>79.000000</v>
       </c>
-      <c r="B80" s="2">
+      <c r="B80" s="0">
         <v>80.000000</v>
       </c>
-      <c r="C80" s="2">
+      <c r="C80" s="0">
         <f>A80+B80</f>
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="2">
+      <c r="A81" s="0">
         <v>80.000000</v>
       </c>
-      <c r="B81" s="2">
+      <c r="B81" s="0">
         <v>81.000000</v>
       </c>
-      <c r="C81" s="2">
+      <c r="C81" s="0">
         <f>A81+B81</f>
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="2">
+      <c r="A82" s="0">
         <v>81.000000</v>
       </c>
-      <c r="B82" s="2">
+      <c r="B82" s="0">
         <v>82.000000</v>
       </c>
-      <c r="C82" s="2">
+      <c r="C82" s="0">
         <f>A82+B82</f>
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="2">
+      <c r="A83" s="0">
         <v>82.000000</v>
       </c>
-      <c r="B83" s="2">
+      <c r="B83" s="0">
         <v>83.000000</v>
       </c>
-      <c r="C83" s="2">
+      <c r="C83" s="0">
         <f>A83+B83</f>
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="2">
+      <c r="A84" s="0">
         <v>83.000000</v>
       </c>
-      <c r="B84" s="2">
+      <c r="B84" s="0">
         <v>84.000000</v>
       </c>
-      <c r="C84" s="2">
+      <c r="C84" s="0">
         <f>A84+B84</f>
       </c>
     </row>
     <row r="85">
-      <c r="A85" s="2">
+      <c r="A85" s="0">
         <v>84.000000</v>
       </c>
-      <c r="B85" s="2">
+      <c r="B85" s="0">
         <v>85.000000</v>
       </c>
-      <c r="C85" s="2">
+      <c r="C85" s="0">
         <f>A85+B85</f>
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="2">
+      <c r="A86" s="0">
         <v>85.000000</v>
       </c>
-      <c r="B86" s="2">
+      <c r="B86" s="0">
         <v>86.000000</v>
       </c>
-      <c r="C86" s="2">
+      <c r="C86" s="0">
         <f>A86+B86</f>
       </c>
     </row>
     <row r="87">
-      <c r="A87" s="2">
+      <c r="A87" s="0">
         <v>86.000000</v>
       </c>
-      <c r="B87" s="2">
+      <c r="B87" s="0">
         <v>87.000000</v>
       </c>
-      <c r="C87" s="2">
+      <c r="C87" s="0">
         <f>A87+B87</f>
       </c>
     </row>
     <row r="88">
-      <c r="A88" s="2">
+      <c r="A88" s="0">
         <v>87.000000</v>
       </c>
-      <c r="B88" s="2">
+      <c r="B88" s="0">
         <v>88.000000</v>
       </c>
-      <c r="C88" s="2">
+      <c r="C88" s="0">
         <f>A88+B88</f>
       </c>
     </row>
     <row r="89">
-      <c r="A89" s="2">
+      <c r="A89" s="0">
         <v>88.000000</v>
       </c>
-      <c r="B89" s="2">
+      <c r="B89" s="0">
         <v>89.000000</v>
       </c>
-      <c r="C89" s="2">
+      <c r="C89" s="0">
         <f>A89+B89</f>
       </c>
     </row>
     <row r="90">
-      <c r="A90" s="2">
+      <c r="A90" s="0">
         <v>89.000000</v>
       </c>
-      <c r="B90" s="2">
+      <c r="B90" s="0">
         <v>90.000000</v>
       </c>
-      <c r="C90" s="2">
+      <c r="C90" s="0">
         <f>A90+B90</f>
       </c>
     </row>
     <row r="91">
-      <c r="A91" s="2">
+      <c r="A91" s="0">
         <v>90.000000</v>
       </c>
-      <c r="B91" s="2">
+      <c r="B91" s="0">
         <v>91.000000</v>
       </c>
-      <c r="C91" s="2">
+      <c r="C91" s="0">
         <f>A91+B91</f>
       </c>
     </row>
     <row r="92">
-      <c r="A92" s="2">
+      <c r="A92" s="0">
         <v>91.000000</v>
       </c>
-      <c r="B92" s="2">
+      <c r="B92" s="0">
         <v>92.000000</v>
       </c>
-      <c r="C92" s="2">
+      <c r="C92" s="0">
         <f>A92+B92</f>
       </c>
     </row>
     <row r="93">
-      <c r="A93" s="2">
+      <c r="A93" s="0">
         <v>92.000000</v>
       </c>
-      <c r="B93" s="2">
+      <c r="B93" s="0">
         <v>93.000000</v>
       </c>
-      <c r="C93" s="2">
+      <c r="C93" s="0">
         <f>A93+B93</f>
       </c>
     </row>
     <row r="94">
-      <c r="A94" s="2">
+      <c r="A94" s="0">
         <v>93.000000</v>
       </c>
-      <c r="B94" s="2">
+      <c r="B94" s="0">
         <v>94.000000</v>
       </c>
-      <c r="C94" s="2">
+      <c r="C94" s="0">
         <f>A94+B94</f>
       </c>
     </row>
     <row r="95">
-      <c r="A95" s="2">
+      <c r="A95" s="0">
         <v>94.000000</v>
       </c>
-      <c r="B95" s="2">
+      <c r="B95" s="0">
         <v>95.000000</v>
       </c>
-      <c r="C95" s="2">
+      <c r="C95" s="0">
         <f>A95+B95</f>
       </c>
     </row>
     <row r="96">
-      <c r="A96" s="2">
+      <c r="A96" s="0">
         <v>95.000000</v>
       </c>
-      <c r="B96" s="2">
+      <c r="B96" s="0">
         <v>96.000000</v>
       </c>
-      <c r="C96" s="2">
+      <c r="C96" s="0">
         <f>A96+B96</f>
       </c>
     </row>
     <row r="97">
-      <c r="A97" s="2">
+      <c r="A97" s="0">
         <v>96.000000</v>
       </c>
-      <c r="B97" s="2">
+      <c r="B97" s="0">
         <v>97.000000</v>
       </c>
-      <c r="C97" s="2">
+      <c r="C97" s="0">
         <f>A97+B97</f>
       </c>
     </row>
     <row r="98">
-      <c r="A98" s="2">
+      <c r="A98" s="0">
         <v>97.000000</v>
       </c>
-      <c r="B98" s="2">
+      <c r="B98" s="0">
         <v>98.000000</v>
       </c>
-      <c r="C98" s="2">
+      <c r="C98" s="0">
         <f>A98+B98</f>
       </c>
     </row>
     <row r="99">
-      <c r="A99" s="2">
+      <c r="A99" s="0">
         <v>98.000000</v>
       </c>
-      <c r="B99" s="2">
+      <c r="B99" s="0">
         <v>99.000000</v>
       </c>
-      <c r="C99" s="2">
+      <c r="C99" s="0">
         <f>A99+B99</f>
       </c>
     </row>
     <row r="100">
-      <c r="A100" s="2">
+      <c r="A100" s="0">
         <v>99.000000</v>
       </c>
-      <c r="B100" s="2">
+      <c r="B100" s="0">
         <v>100.000000</v>
       </c>
-      <c r="C100" s="2">
+      <c r="C100" s="0">
         <f>A100+B100</f>
       </c>
     </row>
     <row r="101">
-      <c r="A101" s="2">
+      <c r="A101" s="0">
         <v>100.000000</v>
       </c>
-      <c r="B101" s="2">
+      <c r="B101" s="0">
         <v>101.000000</v>
       </c>
-      <c r="C101" s="2">
+      <c r="C101" s="0">
         <f>A101+B101</f>
       </c>
     </row>
@@ -1340,7 +1340,7 @@
         </is>
       </c>
       <c r="B102" s="3"/>
-      <c r="C102" s="2">
+      <c r="C102" s="0">
         <f>SUM(C2:C101)</f>
       </c>
     </row>

</xml_diff>